<commit_message>
bringing in update from OneDrive
</commit_message>
<xml_diff>
--- a/models/pinns_worst_of/pinns_worst_of.xlsx
+++ b/models/pinns_worst_of/pinns_worst_of.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f8b2f6c15e78eb2b/Work/ML/PINNs/Worst Of/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{BF192CCB-FC46-4359-9A9C-69B006E91E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B1A5219-DB21-4411-9F3A-A9B2723A84EA}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="13_ncr:1_{BF192CCB-FC46-4359-9A9C-69B006E91E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DABA33B-1660-4707-9F76-CF33FCE6735D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD430F5A-13CC-4C14-99B2-8CFEEE7A8C24}"/>
+    <workbookView xWindow="25320" yWindow="2010" windowWidth="11160" windowHeight="11295" xr2:uid="{DD430F5A-13CC-4C14-99B2-8CFEEE7A8C24}"/>
   </bookViews>
   <sheets>
-    <sheet name="2 assets" sheetId="1" r:id="rId1"/>
+    <sheet name="All data" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="484">
   <si>
     <t>Layers</t>
   </si>
@@ -1271,235 +1272,223 @@
     <t>model_3_assets_20230224-23_18_20</t>
   </si>
   <si>
-    <t>model_4_assets_20230224-23_37_03</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230224-23_47_02</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230224-23_56_58</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-00_06_27</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-00_15_56</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-00_25_21</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-00_34_50</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-00_44_20</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-00_53_30</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-01_02_49</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-01_12_07</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-01_21_34</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-01_30_45</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-01_40_14</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-01_49_44</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-01_59_10</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-02_08_27</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-02_17_44</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-02_27_15</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-02_36_46</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-02_46_19</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-02_55_36</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-03_05_07</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-03_14_42</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-03_24_12</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-03_33_43</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-03_43_06</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-03_52_40</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-04_02_05</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-04_11_26</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-04_21_07</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-04_30_29</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-04_40_04</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-04_49_27</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-04_58_53</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-05_08_23</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-05_17_35</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-05_27_09</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-05_36_26</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-05_46_05</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-05_55_32</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-06_04_58</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-06_14_23</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-06_23_46</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-06_33_09</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-06_42_27</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-06_52_02</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-07_01_31</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-07_11_01</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-07_20_36</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-07_30_19</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-07_39_57</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-07_49_24</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-07_58_53</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-08_08_23</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-08_18_48</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-08_28_46</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-08_38_34</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-08_48_59</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-08_59_42</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-09_11_03</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-09_22_42</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-09_33_09</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-09_43_25</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-09_53_31</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-10_03_21</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-10_13_17</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-10_23_49</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-10_34_09</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-10_44_14</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-10_54_37</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-11_04_48</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-11_15_22</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-11_26_11</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-11_36_04</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-11_45_51</t>
-  </si>
-  <si>
-    <t>model_4_assets_20230225-11_55_40</t>
+    <t>model_4_assets_20230225-18_25_38</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-18_35_34</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-18_45_29</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-18_55_22</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-19_05_11</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-19_15_09</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-19_24_59</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-19_34_44</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-19_45_05</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-19_55_03</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-20_04_53</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-20_14_41</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-20_24_33</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-20_34_32</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-20_44_17</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-20_53_54</t>
+  </si>
+  <si>
+    <t>Epochs</t>
+  </si>
+  <si>
+    <t>Num</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-21_04_18</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-21_14_34</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-21_25_10</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-21_35_31</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-21_46_30</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-21_57_05</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-22_08_12</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-22_18_38</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-22_29_18</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-22_39_59</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Runtime acc.</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-23_22_48</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230225-23_54_33</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-00_26_08</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-00_58_10</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-01_29_49</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-02_00_45</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-02_31_31</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-03_02_02</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-03_33_22</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-04_04_31</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-04_36_01</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-05_07_13</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-05_38_45</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-06_09_16</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-06_40_27</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-07_11_37</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-07_43_12</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-08_13_47</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-08_56_08</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-09_12_18</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-09_28_19</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-09_44_26</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-10_00_20</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-10_16_35</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-10_32_38</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-10_48_50</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-11_05_24</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-11_21_25</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-11_36_55</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-11_52_32</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-12_08_12</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-12_24_08</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-12_40_04</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-12_56_16</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-13_11_51</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-13_27_29</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-13_43_27</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-13_59_08</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-14_14_58</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-14_30_49</t>
+  </si>
+  <si>
+    <t>model_4_assets_20230226-14_46_49</t>
+  </si>
+  <si>
+    <t>Neurons</t>
   </si>
 </sst>
 </file>
@@ -1535,10 +1524,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1554,6 +1544,995 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Runtime perf. vs dimension</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-150"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Summary!$B$4:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Summary!$J$4:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>871.15443596879186</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>857.79282710232656</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1319.0008532958029</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2370.3404115554049</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1717.5430881620184</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2447.9616095228744</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3476.4877386759426</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4697.865993330568</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4983.7698913483573</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13332.822612708351</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8000.3737350976153</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7102.4549632322651</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11353.448010992035</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CF07-4EC8-8943-0831A77EA7C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="394603935"/>
+        <c:axId val="394609343"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="394603935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-150"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="394609343"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="394609343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-150"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="394603935"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-150"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB6BA2CE-C776-544B-AF65-9CD28112A095}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1626,6 +2605,33 @@
     <tableColumn id="1" xr3:uid="{BC8EA318-7AE4-4896-A425-E3A7DEB6A097}" name="Name"/>
     <tableColumn id="2" xr3:uid="{0F584C95-C743-49E2-A95E-1B908FDC5227}" name="Rmse"/>
     <tableColumn id="3" xr3:uid="{196F8BEA-0135-44CD-9FC4-9AA33B23F579}" name="Runtime"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D86FA560-7A25-4F8C-AD8E-5235D5902230}" name="Table6" displayName="Table6" ref="AL12:AN30" totalsRowShown="0">
+  <autoFilter ref="AL12:AN30" xr:uid="{D86FA560-7A25-4F8C-AD8E-5235D5902230}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AL13:AN30">
+    <sortCondition ref="AM12:AM30"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{1E149E04-1F73-4BF0-9944-AA8B0ACA65C3}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{3DBEB3F9-E545-4E2E-A6D7-44F6BE4C9095}" name="Rmse"/>
+    <tableColumn id="3" xr3:uid="{EDD2FB66-4C5A-4A53-B0AD-F6B00EBE9A71}" name="Runtime"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8294C510-7E1F-4701-81A6-0FD25B3B431B}" name="Table7" displayName="Table7" ref="AP12:AR35" totalsRowShown="0">
+  <autoFilter ref="AP12:AR35" xr:uid="{8294C510-7E1F-4701-81A6-0FD25B3B431B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A957CB66-795E-4BF8-AF9B-3F15A900A5D9}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{5C186394-13A0-4606-A052-3C7824482E8D}" name="Rmse"/>
+    <tableColumn id="3" xr3:uid="{EC691BA0-2347-47D0-86C5-5CC0C12C5025}" name="Runtime"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1928,10 +2934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC7701A-9C9C-41E3-ADB6-EFB19D3C9285}">
-  <dimension ref="B2:AJ112"/>
+  <dimension ref="B2:BF112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N7" workbookViewId="0">
-      <selection activeCell="AH31" sqref="AH31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="BF7" sqref="BF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,12 +2963,25 @@
     <col min="26" max="26" width="32" customWidth="1"/>
     <col min="28" max="28" width="10.7109375" customWidth="1"/>
     <col min="29" max="29" width="2.7109375" customWidth="1"/>
+    <col min="32" max="32" width="4.7109375" customWidth="1"/>
     <col min="33" max="33" width="3.5703125" customWidth="1"/>
-    <col min="34" max="34" width="34.5703125" customWidth="1"/>
+    <col min="34" max="34" width="10.140625" customWidth="1"/>
     <col min="36" max="36" width="10.7109375" customWidth="1"/>
+    <col min="37" max="37" width="3" customWidth="1"/>
+    <col min="38" max="38" width="32.5703125" customWidth="1"/>
+    <col min="40" max="40" width="10.7109375" customWidth="1"/>
+    <col min="41" max="41" width="3.5703125" customWidth="1"/>
+    <col min="42" max="44" width="12.28515625" customWidth="1"/>
+    <col min="45" max="45" width="3.5703125" customWidth="1"/>
+    <col min="46" max="46" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.7109375" customWidth="1"/>
+    <col min="48" max="48" width="6.5703125" customWidth="1"/>
+    <col min="49" max="49" width="3.5703125" customWidth="1"/>
+    <col min="52" max="52" width="3.42578125" customWidth="1"/>
+    <col min="53" max="53" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>205</v>
       </c>
@@ -2005,14 +3024,56 @@
       <c r="AA2">
         <v>3</v>
       </c>
+      <c r="AD2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE2">
+        <v>3</v>
+      </c>
       <c r="AH2" t="s">
         <v>205</v>
       </c>
       <c r="AI2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM2">
+        <v>4</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ2">
+        <v>4</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AU2">
+        <v>5</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AY2">
+        <v>5</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BC2">
+        <v>5</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BF2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -2055,14 +3116,56 @@
       <c r="AA3">
         <v>4</v>
       </c>
+      <c r="AD3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>4</v>
+      </c>
       <c r="AH3" t="s">
         <v>0</v>
       </c>
       <c r="AI3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AL3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>4</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>4</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>4</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>4</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC3">
+        <v>4</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -2105,14 +3208,53 @@
       <c r="AA4">
         <v>10</v>
       </c>
+      <c r="AD4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE4">
+        <v>20</v>
+      </c>
       <c r="AH4" t="s">
         <v>1</v>
       </c>
       <c r="AI4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AL4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM4">
+        <v>20</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ4">
+        <v>10</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY4">
+        <v>20</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC4">
+        <v>20</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>206</v>
       </c>
@@ -2155,14 +3297,53 @@
       <c r="AA5">
         <v>6</v>
       </c>
+      <c r="AD5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE5">
+        <v>6</v>
+      </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AL5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AM5">
+        <v>10</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AQ5">
+        <v>10</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AY5">
+        <v>6</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>206</v>
+      </c>
+      <c r="BC5">
+        <v>10</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>206</v>
+      </c>
+      <c r="BF5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>307</v>
       </c>
@@ -2212,15 +3393,56 @@
         <f>AVERAGE(Table4[Rmse])</f>
         <v>46.057377165327679</v>
       </c>
+      <c r="AD6" t="s">
+        <v>307</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>41.66</v>
+      </c>
       <c r="AH6" t="s">
         <v>307</v>
       </c>
       <c r="AI6" s="1">
         <f>AVERAGE(Table5[Rmse])</f>
-        <v>23.926255426509275</v>
-      </c>
-    </row>
-    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
+        <v>88.348388835249494</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>307</v>
+      </c>
+      <c r="AM6" s="1">
+        <f>AVERAGE(Table6[Rmse])</f>
+        <v>45.45223578363229</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>307</v>
+      </c>
+      <c r="AQ6" s="1">
+        <f>AVERAGE(Table7[Rmse])</f>
+        <v>73.905803199189606</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>307</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>307</v>
+      </c>
+      <c r="AY6" s="1">
+        <v>101.27</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>307</v>
+      </c>
+      <c r="BC6" s="1">
+        <v>93.6</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>483</v>
+      </c>
+      <c r="BF6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>308</v>
       </c>
@@ -2270,15 +3492,56 @@
         <f>_xlfn.STDEV.P(Table4[Rmse])</f>
         <v>39.177779337550547</v>
       </c>
+      <c r="AD7" t="s">
+        <v>308</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>34.56</v>
+      </c>
       <c r="AH7" t="s">
         <v>308</v>
       </c>
       <c r="AI7" s="1">
         <f>_xlfn.STDEV.P(Table5[Rmse])</f>
-        <v>33.693508323290395</v>
-      </c>
-    </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
+        <v>51.712982041973994</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>308</v>
+      </c>
+      <c r="AM7" s="1">
+        <f>_xlfn.STDEV.P(Table6[Rmse])</f>
+        <v>28.525833152605127</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>308</v>
+      </c>
+      <c r="AQ7" s="1">
+        <f>_xlfn.STDEV.P(Table7[Rmse])</f>
+        <v>68.532048385325467</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>308</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>308</v>
+      </c>
+      <c r="AY7" s="1">
+        <v>46.88</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>308</v>
+      </c>
+      <c r="BC7" s="1">
+        <v>53.08</v>
+      </c>
+      <c r="BE7" t="s">
+        <v>307</v>
+      </c>
+      <c r="BF7" s="1">
+        <v>83.62</v>
+      </c>
+    </row>
+    <row r="8" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>309</v>
       </c>
@@ -2328,15 +3591,56 @@
         <f>MIN(Table4[Rmse])</f>
         <v>9.35779890535931</v>
       </c>
+      <c r="AD8" t="s">
+        <v>309</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>8.56</v>
+      </c>
       <c r="AH8" t="s">
         <v>309</v>
       </c>
       <c r="AI8" s="1">
         <f>MIN(Table5[Rmse])</f>
-        <v>4.0891620367546198</v>
-      </c>
-    </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
+        <v>21.796768845109401</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>309</v>
+      </c>
+      <c r="AM8" s="1">
+        <f>MIN(Table6[Rmse])</f>
+        <v>7.6302622165553098</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>309</v>
+      </c>
+      <c r="AQ8" s="1">
+        <f>MIN(Table7[Rmse])</f>
+        <v>12.4246888568565</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>309</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>309</v>
+      </c>
+      <c r="AY8" s="1">
+        <v>45.49</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>309</v>
+      </c>
+      <c r="BC8" s="1">
+        <v>29.84</v>
+      </c>
+      <c r="BE8" t="s">
+        <v>308</v>
+      </c>
+      <c r="BF8" s="1">
+        <v>48.69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>310</v>
       </c>
@@ -2386,15 +3690,56 @@
         <f>MAX(Table4[Rmse])</f>
         <v>202.02761392331701</v>
       </c>
+      <c r="AD9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>208.96</v>
+      </c>
       <c r="AH9" t="s">
         <v>310</v>
       </c>
       <c r="AI9" s="1">
         <f>MAX(Table5[Rmse])</f>
-        <v>266.75183048566703</v>
-      </c>
-    </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
+        <v>189.913998443948</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AM9" s="1">
+        <f>MAX(Table6[Rmse])</f>
+        <v>109.48538512603299</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AQ9" s="1">
+        <f>MAX(Table7[Rmse])</f>
+        <v>262.73554063072402</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AY9" s="1">
+        <v>223.26</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>310</v>
+      </c>
+      <c r="BC9" s="1">
+        <v>208.7</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>309</v>
+      </c>
+      <c r="BF9" s="1">
+        <v>18.05</v>
+      </c>
+    </row>
+    <row r="10" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -2444,15 +3789,64 @@
         <f>AVERAGE(Table4[Runtime])</f>
         <v>463.65548329353317</v>
       </c>
+      <c r="AD10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>646</v>
+      </c>
       <c r="AH10" t="s">
         <v>4</v>
       </c>
       <c r="AI10" s="2">
         <f>AVERAGE(Table5[Runtime])</f>
-        <v>565.15281880985594</v>
-      </c>
-    </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
+        <v>591.40521828944838</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM10" s="2">
+        <f>AVERAGE(Table6[Runtime])</f>
+        <v>1860.1847903066159</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ10" s="2">
+        <f>AVERAGE(Table7[Runtime])</f>
+        <v>937.89995930505825</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY10" s="2">
+        <v>839</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC10" s="2">
+        <v>1334</v>
+      </c>
+      <c r="BE10" t="s">
+        <v>310</v>
+      </c>
+      <c r="BF10" s="1">
+        <v>223.76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:58" x14ac:dyDescent="0.25">
+      <c r="BE11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF11" s="2">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="12" spans="2:58" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
         <v>2</v>
       </c>
@@ -2498,8 +3892,26 @@
       <c r="AJ12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AL12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:58" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
         <v>39</v>
       </c>
@@ -2537,16 +3949,34 @@
         <v>463.398053884506</v>
       </c>
       <c r="AH13" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="AI13">
-        <v>4.0891620367546198</v>
+        <v>167.37266630948901</v>
       </c>
       <c r="AJ13">
-        <v>539.207851409912</v>
-      </c>
-    </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
+        <v>589.99266886711098</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>448</v>
+      </c>
+      <c r="AM13">
+        <v>7.6302622165553098</v>
+      </c>
+      <c r="AN13">
+        <v>1827.73245978355</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>460</v>
+      </c>
+      <c r="AQ13">
+        <v>115.15316213091999</v>
+      </c>
+      <c r="AR13">
+        <v>948.78363347053505</v>
+      </c>
+    </row>
+    <row r="14" spans="2:58" x14ac:dyDescent="0.25">
       <c r="J14" t="s">
         <v>80</v>
       </c>
@@ -2584,16 +4014,34 @@
         <v>453.58618712425198</v>
       </c>
       <c r="AH14" t="s">
-        <v>442</v>
+        <v>412</v>
       </c>
       <c r="AI14">
-        <v>4.3062052686741996</v>
+        <v>49.976348178406603</v>
       </c>
       <c r="AJ14">
-        <v>545.123963832855</v>
-      </c>
-    </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
+        <v>576.63890051841702</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>451</v>
+      </c>
+      <c r="AM14">
+        <v>13.0392217630123</v>
+      </c>
+      <c r="AN14">
+        <v>1850.38824057579</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>461</v>
+      </c>
+      <c r="AQ14">
+        <v>41.582172066565903</v>
+      </c>
+      <c r="AR14">
+        <v>950.03967452049199</v>
+      </c>
+    </row>
+    <row r="15" spans="2:58" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
         <v>64</v>
       </c>
@@ -2631,16 +4079,34 @@
         <v>459.121977090835</v>
       </c>
       <c r="AH15" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="AI15">
-        <v>4.3223931583762001</v>
+        <v>57.0512766968655</v>
       </c>
       <c r="AJ15">
-        <v>554.36101341247502</v>
-      </c>
-    </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
+        <v>576.596893548965</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>445</v>
+      </c>
+      <c r="AM15">
+        <v>15.0864942667565</v>
+      </c>
+      <c r="AN15">
+        <v>1900.8211030959999</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>462</v>
+      </c>
+      <c r="AQ15">
+        <v>35.2875550181001</v>
+      </c>
+      <c r="AR15">
+        <v>941.15254831313996</v>
+      </c>
+    </row>
+    <row r="16" spans="2:58" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>98</v>
       </c>
@@ -2678,16 +4144,34 @@
         <v>477.76753211021401</v>
       </c>
       <c r="AH16" t="s">
-        <v>478</v>
+        <v>414</v>
       </c>
       <c r="AI16">
-        <v>5.1897451236248502</v>
+        <v>76.778461834606006</v>
       </c>
       <c r="AJ16">
-        <v>606.12848806381203</v>
-      </c>
-    </row>
-    <row r="17" spans="10:36" x14ac:dyDescent="0.25">
+        <v>574.13170123100201</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>444</v>
+      </c>
+      <c r="AM16">
+        <v>22.2025824897894</v>
+      </c>
+      <c r="AN16">
+        <v>1875.1054179668399</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>463</v>
+      </c>
+      <c r="AQ16">
+        <v>48.644646449863899</v>
+      </c>
+      <c r="AR16">
+        <v>949.33190155029297</v>
+      </c>
+    </row>
+    <row r="17" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>92</v>
       </c>
@@ -2725,16 +4209,34 @@
         <v>463.04531097412098</v>
       </c>
       <c r="AH17" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="AI17">
-        <v>5.5904933790990201</v>
+        <v>184.94094263844201</v>
       </c>
       <c r="AJ17">
-        <v>540.74134016036896</v>
-      </c>
-    </row>
-    <row r="18" spans="10:36" x14ac:dyDescent="0.25">
+        <v>571.24462223052899</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>453</v>
+      </c>
+      <c r="AM17">
+        <v>24.708956476632501</v>
+      </c>
+      <c r="AN17">
+        <v>1853.10335588455</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>464</v>
+      </c>
+      <c r="AQ17">
+        <v>34.965195797449297</v>
+      </c>
+      <c r="AR17">
+        <v>935.95018720626797</v>
+      </c>
+    </row>
+    <row r="18" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>93</v>
       </c>
@@ -2772,16 +4274,34 @@
         <v>440.219444274902</v>
       </c>
       <c r="AH18" t="s">
-        <v>472</v>
+        <v>416</v>
       </c>
       <c r="AI18">
-        <v>5.6648059320352901</v>
+        <v>72.153930098329198</v>
       </c>
       <c r="AJ18">
-        <v>678.36032509803704</v>
-      </c>
-    </row>
-    <row r="19" spans="10:36" x14ac:dyDescent="0.25">
+        <v>579.56695222854603</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>447</v>
+      </c>
+      <c r="AM18">
+        <v>24.893005124852301</v>
+      </c>
+      <c r="AN18">
+        <v>1837.0055143833099</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>465</v>
+      </c>
+      <c r="AQ18">
+        <v>245.681989465979</v>
+      </c>
+      <c r="AR18">
+        <v>955.21150279045105</v>
+      </c>
+    </row>
+    <row r="19" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
         <v>75</v>
       </c>
@@ -2819,16 +4339,34 @@
         <v>480.72208690643299</v>
       </c>
       <c r="AH19" t="s">
-        <v>485</v>
+        <v>417</v>
       </c>
       <c r="AI19">
-        <v>5.7069507590962303</v>
+        <v>183.47851898495901</v>
       </c>
       <c r="AJ19">
-        <v>574.32763886451698</v>
-      </c>
-    </row>
-    <row r="20" spans="10:36" x14ac:dyDescent="0.25">
+        <v>570.58983230590798</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>449</v>
+      </c>
+      <c r="AM19">
+        <v>27.499515478880099</v>
+      </c>
+      <c r="AN19">
+        <v>1812.6312959194099</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>466</v>
+      </c>
+      <c r="AQ19">
+        <v>26.1258874920645</v>
+      </c>
+      <c r="AR19">
+        <v>944.97830390930096</v>
+      </c>
+    </row>
+    <row r="20" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
         <v>55</v>
       </c>
@@ -2866,16 +4404,34 @@
         <v>460.83387351035998</v>
       </c>
       <c r="AH20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AI20">
-        <v>5.7279088773814104</v>
+        <v>21.796768845109401</v>
       </c>
       <c r="AJ20">
-        <v>533.662622451782</v>
-      </c>
-    </row>
-    <row r="21" spans="10:36" x14ac:dyDescent="0.25">
+        <v>565.84134793281498</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>443</v>
+      </c>
+      <c r="AM20">
+        <v>34.387965491025099</v>
+      </c>
+      <c r="AN20">
+        <v>1884.20600843429</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>467</v>
+      </c>
+      <c r="AQ20">
+        <v>72.9404942033336</v>
+      </c>
+      <c r="AR20">
+        <v>953.10570979118302</v>
+      </c>
+    </row>
+    <row r="21" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
         <v>52</v>
       </c>
@@ -2913,16 +4469,34 @@
         <v>460.43400025367703</v>
       </c>
       <c r="AH21" t="s">
-        <v>487</v>
+        <v>419</v>
       </c>
       <c r="AI21">
-        <v>5.8501714773277396</v>
+        <v>31.793441624102002</v>
       </c>
       <c r="AJ21">
-        <v>570.71277117729096</v>
-      </c>
-    </row>
-    <row r="22" spans="10:36" x14ac:dyDescent="0.25">
+        <v>602.99255466461102</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>442</v>
+      </c>
+      <c r="AM21">
+        <v>36.389769592881301</v>
+      </c>
+      <c r="AN21">
+        <v>1949.94825649261</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>468</v>
+      </c>
+      <c r="AQ21">
+        <v>120.65689528749</v>
+      </c>
+      <c r="AR21">
+        <v>975.75802922248795</v>
+      </c>
+    </row>
+    <row r="22" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
         <v>25</v>
       </c>
@@ -2960,16 +4534,34 @@
         <v>512.01895260810795</v>
       </c>
       <c r="AH22" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="AI22">
-        <v>7.3133214838763196</v>
+        <v>57.971851883797399</v>
       </c>
       <c r="AJ22">
-        <v>552.19868206977799</v>
-      </c>
-    </row>
-    <row r="23" spans="10:36" x14ac:dyDescent="0.25">
+        <v>579.19907498359601</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>452</v>
+      </c>
+      <c r="AM22">
+        <v>43.985161591836203</v>
+      </c>
+      <c r="AN22">
+        <v>1870.9016826152799</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>469</v>
+      </c>
+      <c r="AQ22">
+        <v>56.1235676931841</v>
+      </c>
+      <c r="AR22">
+        <v>941.90426778793301</v>
+      </c>
+    </row>
+    <row r="23" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
         <v>12</v>
       </c>
@@ -3007,16 +4599,34 @@
         <v>430.98987317085198</v>
       </c>
       <c r="AH23" t="s">
+        <v>421</v>
+      </c>
+      <c r="AI23">
+        <v>189.913998443948</v>
+      </c>
+      <c r="AJ23">
+        <v>571.13665747642494</v>
+      </c>
+      <c r="AL23" t="s">
         <v>455</v>
       </c>
-      <c r="AI23">
-        <v>7.4535165018506602</v>
-      </c>
-      <c r="AJ23">
-        <v>544.88103985786404</v>
-      </c>
-    </row>
-    <row r="24" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="AM23">
+        <v>46.881006810166099</v>
+      </c>
+      <c r="AN23">
+        <v>1811.7425656318601</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>470</v>
+      </c>
+      <c r="AQ23">
+        <v>262.73554063072402</v>
+      </c>
+      <c r="AR23">
+        <v>912.94152522087097</v>
+      </c>
+    </row>
+    <row r="24" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
         <v>97</v>
       </c>
@@ -3054,16 +4664,34 @@
         <v>468.86631035804697</v>
       </c>
       <c r="AH24" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
       <c r="AI24">
-        <v>7.4985319894394404</v>
+        <v>82.052084004086097</v>
       </c>
       <c r="AJ24">
-        <v>549.13167238235405</v>
-      </c>
-    </row>
-    <row r="25" spans="10:36" x14ac:dyDescent="0.25">
+        <v>570.59081888198796</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>450</v>
+      </c>
+      <c r="AM24">
+        <v>47.073675471259797</v>
+      </c>
+      <c r="AN24">
+        <v>1860.72394204139</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>471</v>
+      </c>
+      <c r="AQ24">
+        <v>36.567508964266402</v>
+      </c>
+      <c r="AR24">
+        <v>918.010901927948</v>
+      </c>
+    </row>
+    <row r="25" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
         <v>38</v>
       </c>
@@ -3101,16 +4729,34 @@
         <v>450.63516569137499</v>
       </c>
       <c r="AH25" t="s">
-        <v>471</v>
+        <v>423</v>
       </c>
       <c r="AI25">
-        <v>7.5041358877872604</v>
+        <v>130.38552249038199</v>
       </c>
       <c r="AJ25">
-        <v>646.34873986244202</v>
-      </c>
-    </row>
-    <row r="26" spans="10:36" x14ac:dyDescent="0.25">
+        <v>573.74280714988697</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>459</v>
+      </c>
+      <c r="AM25">
+        <v>47.9935183627342</v>
+      </c>
+      <c r="AN25">
+        <v>1816.34609580039</v>
+      </c>
+      <c r="AP25" t="s">
+        <v>472</v>
+      </c>
+      <c r="AQ25">
+        <v>15.114148393215499</v>
+      </c>
+      <c r="AR25">
+        <v>922.69541811942997</v>
+      </c>
+    </row>
+    <row r="26" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
         <v>49</v>
       </c>
@@ -3148,16 +4794,34 @@
         <v>455.62053751945399</v>
       </c>
       <c r="AH26" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="AI26">
-        <v>7.7839706467930903</v>
+        <v>52.672394795735499</v>
       </c>
       <c r="AJ26">
-        <v>552.97345590591397</v>
-      </c>
-    </row>
-    <row r="27" spans="10:36" x14ac:dyDescent="0.25">
+        <v>574.40559935569695</v>
+      </c>
+      <c r="AL26" t="s">
+        <v>456</v>
+      </c>
+      <c r="AM26">
+        <v>60.336952859441503</v>
+      </c>
+      <c r="AN26">
+        <v>1852.2056474685601</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>473</v>
+      </c>
+      <c r="AQ26">
+        <v>21.281010267749998</v>
+      </c>
+      <c r="AR26">
+        <v>936.07313370704605</v>
+      </c>
+    </row>
+    <row r="27" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J27" t="s">
         <v>26</v>
       </c>
@@ -3195,16 +4859,34 @@
         <v>446.30051231384198</v>
       </c>
       <c r="AH27" t="s">
-        <v>461</v>
+        <v>425</v>
       </c>
       <c r="AI27">
-        <v>8.2347232194394806</v>
+        <v>107.66744444236799</v>
       </c>
       <c r="AJ27">
-        <v>565.72738623619</v>
-      </c>
-    </row>
-    <row r="28" spans="10:36" x14ac:dyDescent="0.25">
+        <v>566.78603672981205</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>454</v>
+      </c>
+      <c r="AM27">
+        <v>78.799314650829601</v>
+      </c>
+      <c r="AN27">
+        <v>1873.50085163116</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>474</v>
+      </c>
+      <c r="AQ27">
+        <v>40.338673002617902</v>
+      </c>
+      <c r="AR27">
+        <v>930.30697607994</v>
+      </c>
+    </row>
+    <row r="28" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J28" t="s">
         <v>88</v>
       </c>
@@ -3242,16 +4924,34 @@
         <v>430.25905394554098</v>
       </c>
       <c r="AH28" t="s">
-        <v>477</v>
+        <v>426</v>
       </c>
       <c r="AI28">
-        <v>8.2618091878719007</v>
+        <v>84.399228715947402</v>
       </c>
       <c r="AJ28">
-        <v>575.75918126106205</v>
-      </c>
-    </row>
-    <row r="29" spans="10:36" x14ac:dyDescent="0.25">
+        <v>559.21046495437599</v>
+      </c>
+      <c r="AL28" t="s">
+        <v>458</v>
+      </c>
+      <c r="AM28">
+        <v>81.610281153570398</v>
+      </c>
+      <c r="AN28">
+        <v>1876.12600588798</v>
+      </c>
+      <c r="AP28" t="s">
+        <v>475</v>
+      </c>
+      <c r="AQ28">
+        <v>57.292404639778397</v>
+      </c>
+      <c r="AR28">
+        <v>953.22767472267105</v>
+      </c>
+    </row>
+    <row r="29" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J29" t="s">
         <v>10</v>
       </c>
@@ -3289,16 +4989,34 @@
         <v>539.31304001808098</v>
       </c>
       <c r="AH29" t="s">
-        <v>449</v>
+        <v>429</v>
       </c>
       <c r="AI29">
-        <v>8.9595451026719903</v>
+        <v>92.559397808644505</v>
       </c>
       <c r="AJ29">
-        <v>539.07887935638405</v>
-      </c>
-    </row>
-    <row r="30" spans="10:36" x14ac:dyDescent="0.25">
+        <v>606.39481377601601</v>
+      </c>
+      <c r="AL29" t="s">
+        <v>457</v>
+      </c>
+      <c r="AM29">
+        <v>96.137175179125606</v>
+      </c>
+      <c r="AN29">
+        <v>1851.2799568176199</v>
+      </c>
+      <c r="AP29" t="s">
+        <v>476</v>
+      </c>
+      <c r="AQ29">
+        <v>194.807320326514</v>
+      </c>
+      <c r="AR29">
+        <v>916.71532917022705</v>
+      </c>
+    </row>
+    <row r="30" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J30" t="s">
         <v>27</v>
       </c>
@@ -3336,16 +5054,34 @@
         <v>457.52076196670498</v>
       </c>
       <c r="AH30" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="AI30">
-        <v>9.1661928589810397</v>
+        <v>26.807145243188799</v>
       </c>
       <c r="AJ30">
-        <v>556.65925979614201</v>
-      </c>
-    </row>
-    <row r="31" spans="10:36" x14ac:dyDescent="0.25">
+        <v>594.13731479644696</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>446</v>
+      </c>
+      <c r="AM30">
+        <v>109.48538512603299</v>
+      </c>
+      <c r="AN30">
+        <v>1879.5578250885001</v>
+      </c>
+      <c r="AP30" t="s">
+        <v>477</v>
+      </c>
+      <c r="AQ30">
+        <v>48.910451113979803</v>
+      </c>
+      <c r="AR30">
+        <v>917.71700787544205</v>
+      </c>
+    </row>
+    <row r="31" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
         <v>74</v>
       </c>
@@ -3383,16 +5119,25 @@
         <v>455.89282536506602</v>
       </c>
       <c r="AH31" t="s">
-        <v>468</v>
+        <v>431</v>
       </c>
       <c r="AI31">
-        <v>9.2769960390423893</v>
+        <v>83.622378227687193</v>
       </c>
       <c r="AJ31">
-        <v>570.13297963142395</v>
-      </c>
-    </row>
-    <row r="32" spans="10:36" x14ac:dyDescent="0.25">
+        <v>615.95134997367802</v>
+      </c>
+      <c r="AP31" t="s">
+        <v>478</v>
+      </c>
+      <c r="AQ31">
+        <v>21.195203637780899</v>
+      </c>
+      <c r="AR31">
+        <v>938.48336482048001</v>
+      </c>
+    </row>
+    <row r="32" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J32" t="s">
         <v>63</v>
       </c>
@@ -3430,16 +5175,25 @@
         <v>474.82596969604401</v>
       </c>
       <c r="AH32" t="s">
-        <v>484</v>
+        <v>432</v>
       </c>
       <c r="AI32">
-        <v>9.3821319662645806</v>
+        <v>50.335431043255099</v>
       </c>
       <c r="AJ32">
-        <v>629.51316165924004</v>
-      </c>
-    </row>
-    <row r="33" spans="10:36" x14ac:dyDescent="0.25">
+        <v>603.040471315383</v>
+      </c>
+      <c r="AP32" t="s">
+        <v>479</v>
+      </c>
+      <c r="AQ32">
+        <v>12.4246888568565</v>
+      </c>
+      <c r="AR32">
+        <v>924.36787509918202</v>
+      </c>
+    </row>
+    <row r="33" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J33" t="s">
         <v>41</v>
       </c>
@@ -3477,16 +5231,25 @@
         <v>449.58346390724103</v>
       </c>
       <c r="AH33" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="AI33">
-        <v>9.6232284181680594</v>
+        <v>61.521291584156202</v>
       </c>
       <c r="AJ33">
-        <v>551.52591943740799</v>
-      </c>
-    </row>
-    <row r="34" spans="10:36" x14ac:dyDescent="0.25">
+        <v>640.47252082824696</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>480</v>
+      </c>
+      <c r="AQ33">
+        <v>61.938839622774303</v>
+      </c>
+      <c r="AR33">
+        <v>930.73285293579102</v>
+      </c>
+    </row>
+    <row r="34" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J34" t="s">
         <v>65</v>
       </c>
@@ -3524,16 +5287,25 @@
         <v>450.99981355667097</v>
       </c>
       <c r="AH34" t="s">
-        <v>462</v>
+        <v>434</v>
       </c>
       <c r="AI34">
-        <v>9.8317986046965498</v>
+        <v>47.615420715563999</v>
       </c>
       <c r="AJ34">
-        <v>560.64900636672905</v>
-      </c>
-    </row>
-    <row r="35" spans="10:36" x14ac:dyDescent="0.25">
+        <v>616.736087560653</v>
+      </c>
+      <c r="AP34" t="s">
+        <v>481</v>
+      </c>
+      <c r="AQ34">
+        <v>48.335661743141898</v>
+      </c>
+      <c r="AR34">
+        <v>932.94014811515797</v>
+      </c>
+    </row>
+    <row r="35" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J35" t="s">
         <v>83</v>
       </c>
@@ -3571,16 +5343,25 @@
         <v>446.64840149879399</v>
       </c>
       <c r="AH35" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="AI35">
-        <v>9.9275036995451007</v>
+        <v>58.761677396127801</v>
       </c>
       <c r="AJ35">
-        <v>563.06321406364395</v>
-      </c>
-    </row>
-    <row r="36" spans="10:36" x14ac:dyDescent="0.25">
+        <v>647.46031570434502</v>
+      </c>
+      <c r="AP35" t="s">
+        <v>482</v>
+      </c>
+      <c r="AQ35">
+        <v>81.7304567770109</v>
+      </c>
+      <c r="AR35">
+        <v>941.27109766006402</v>
+      </c>
+    </row>
+    <row r="36" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J36" t="s">
         <v>7</v>
       </c>
@@ -3618,16 +5399,16 @@
         <v>427.831951379776</v>
       </c>
       <c r="AH36" t="s">
-        <v>479</v>
+        <v>436</v>
       </c>
       <c r="AI36">
-        <v>9.9372874686490196</v>
+        <v>174.822783268188</v>
       </c>
       <c r="AJ36">
-        <v>599.82548475265503</v>
-      </c>
-    </row>
-    <row r="37" spans="10:36" x14ac:dyDescent="0.25">
+        <v>606.32495880126896</v>
+      </c>
+    </row>
+    <row r="37" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J37" t="s">
         <v>69</v>
       </c>
@@ -3665,16 +5446,16 @@
         <v>463.72971439361498</v>
       </c>
       <c r="AH37" t="s">
-        <v>464</v>
+        <v>437</v>
       </c>
       <c r="AI37">
-        <v>11.3801166209455</v>
+        <v>116.40306277243199</v>
       </c>
       <c r="AJ37">
-        <v>551.15801835060097</v>
-      </c>
-    </row>
-    <row r="38" spans="10:36" x14ac:dyDescent="0.25">
+        <v>622.10690212249699</v>
+      </c>
+    </row>
+    <row r="38" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J38" t="s">
         <v>14</v>
       </c>
@@ -3712,16 +5493,16 @@
         <v>433.83012914657502</v>
       </c>
       <c r="AH38" t="s">
-        <v>482</v>
+        <v>438</v>
       </c>
       <c r="AI38">
-        <v>11.408372789812599</v>
+        <v>34.204641670670298</v>
       </c>
       <c r="AJ38">
-        <v>591.768070936203</v>
-      </c>
-    </row>
-    <row r="39" spans="10:36" x14ac:dyDescent="0.25">
+        <v>621.24400758743195</v>
+      </c>
+    </row>
+    <row r="39" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J39" t="s">
         <v>51</v>
       </c>
@@ -3758,17 +5539,8 @@
       <c r="AB39">
         <v>457.357856750488</v>
       </c>
-      <c r="AH39" t="s">
-        <v>481</v>
-      </c>
-      <c r="AI39">
-        <v>11.546790460520199</v>
-      </c>
-      <c r="AJ39">
-        <v>603.01647877693097</v>
-      </c>
-    </row>
-    <row r="40" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J40" t="s">
         <v>101</v>
       </c>
@@ -3805,17 +5577,8 @@
       <c r="AB40">
         <v>474.09562969207701</v>
       </c>
-      <c r="AH40" t="s">
-        <v>440</v>
-      </c>
-      <c r="AI40">
-        <v>11.649365947830701</v>
-      </c>
-      <c r="AJ40">
-        <v>543.19556188583294</v>
-      </c>
-    </row>
-    <row r="41" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J41" t="s">
         <v>6</v>
       </c>
@@ -3852,17 +5615,8 @@
       <c r="AB41">
         <v>456.19778966903601</v>
       </c>
-      <c r="AH41" t="s">
-        <v>474</v>
-      </c>
-      <c r="AI41">
-        <v>11.9683194096176</v>
-      </c>
-      <c r="AJ41">
-        <v>597.93063735961903</v>
-      </c>
-    </row>
-    <row r="42" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
         <v>86</v>
       </c>
@@ -3899,17 +5653,8 @@
       <c r="AB42">
         <v>462.59431123733498</v>
       </c>
-      <c r="AH42" t="s">
-        <v>444</v>
-      </c>
-      <c r="AI42">
-        <v>12.3411781121179</v>
-      </c>
-      <c r="AJ42">
-        <v>545.09297299385003</v>
-      </c>
-    </row>
-    <row r="43" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J43" t="s">
         <v>91</v>
       </c>
@@ -3946,17 +5691,8 @@
       <c r="AB43">
         <v>455.73748636245699</v>
       </c>
-      <c r="AH43" t="s">
-        <v>452</v>
-      </c>
-      <c r="AI43">
-        <v>12.3501145859774</v>
-      </c>
-      <c r="AJ43">
-        <v>548.89375805854797</v>
-      </c>
-    </row>
-    <row r="44" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J44" t="s">
         <v>79</v>
       </c>
@@ -3993,17 +5729,8 @@
       <c r="AB44">
         <v>449.81938934326098</v>
       </c>
-      <c r="AH44" t="s">
-        <v>483</v>
-      </c>
-      <c r="AI44">
-        <v>12.6523279758963</v>
-      </c>
-      <c r="AJ44">
-        <v>614.27499079704205</v>
-      </c>
-    </row>
-    <row r="45" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J45" t="s">
         <v>99</v>
       </c>
@@ -4040,17 +5767,8 @@
       <c r="AB45">
         <v>579.83819842338505</v>
       </c>
-      <c r="AH45" t="s">
-        <v>447</v>
-      </c>
-      <c r="AI45">
-        <v>13.203035062382799</v>
-      </c>
-      <c r="AJ45">
-        <v>534.90922284126202</v>
-      </c>
-    </row>
-    <row r="46" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J46" t="s">
         <v>61</v>
       </c>
@@ -4087,17 +5805,8 @@
       <c r="AB46">
         <v>448.00596833229002</v>
       </c>
-      <c r="AH46" t="s">
-        <v>439</v>
-      </c>
-      <c r="AI46">
-        <v>13.963577691539101</v>
-      </c>
-      <c r="AJ46">
-        <v>548.20696568488995</v>
-      </c>
-    </row>
-    <row r="47" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J47" t="s">
         <v>46</v>
       </c>
@@ -4134,17 +5843,8 @@
       <c r="AB47">
         <v>495.796495914459</v>
       </c>
-      <c r="AH47" t="s">
-        <v>416</v>
-      </c>
-      <c r="AI47">
-        <v>14.160924784261001</v>
-      </c>
-      <c r="AJ47">
-        <v>547.71113562583901</v>
-      </c>
-    </row>
-    <row r="48" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="10:44" x14ac:dyDescent="0.25">
       <c r="J48" t="s">
         <v>87</v>
       </c>
@@ -4181,17 +5881,8 @@
       <c r="AB48">
         <v>448.52136564254698</v>
       </c>
-      <c r="AH48" t="s">
-        <v>415</v>
-      </c>
-      <c r="AI48">
-        <v>14.447627982771101</v>
-      </c>
-      <c r="AJ48">
-        <v>550.72817349433899</v>
-      </c>
-    </row>
-    <row r="49" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J49" t="s">
         <v>36</v>
       </c>
@@ -4228,17 +5919,8 @@
       <c r="AB49">
         <v>459.59826707839898</v>
       </c>
-      <c r="AH49" t="s">
-        <v>467</v>
-      </c>
-      <c r="AI49">
-        <v>14.7517294316654</v>
-      </c>
-      <c r="AJ49">
-        <v>577.01978063583294</v>
-      </c>
-    </row>
-    <row r="50" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J50" t="s">
         <v>31</v>
       </c>
@@ -4275,17 +5957,8 @@
       <c r="AB50">
         <v>451.35959744453402</v>
       </c>
-      <c r="AH50" t="s">
-        <v>460</v>
-      </c>
-      <c r="AI50">
-        <v>15.2972842284991</v>
-      </c>
-      <c r="AJ50">
-        <v>557.26708555221501</v>
-      </c>
-    </row>
-    <row r="51" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J51" t="s">
         <v>42</v>
       </c>
@@ -4322,17 +5995,8 @@
       <c r="AB51">
         <v>452.07966899871798</v>
       </c>
-      <c r="AH51" t="s">
-        <v>412</v>
-      </c>
-      <c r="AI51">
-        <v>15.698199250781601</v>
-      </c>
-      <c r="AJ51">
-        <v>580.11878943443298</v>
-      </c>
-    </row>
-    <row r="52" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J52" t="s">
         <v>28</v>
       </c>
@@ -4369,17 +6033,8 @@
       <c r="AB52">
         <v>464.61766505241297</v>
       </c>
-      <c r="AH52" t="s">
-        <v>456</v>
-      </c>
-      <c r="AI52">
-        <v>15.915390711966699</v>
-      </c>
-      <c r="AJ52">
-        <v>541.49011397361699</v>
-      </c>
-    </row>
-    <row r="53" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J53" t="s">
         <v>32</v>
       </c>
@@ -4416,17 +6071,8 @@
       <c r="AB53">
         <v>448.66396808624199</v>
       </c>
-      <c r="AH53" t="s">
-        <v>475</v>
-      </c>
-      <c r="AI53">
-        <v>16.470292499913501</v>
-      </c>
-      <c r="AJ53">
-        <v>586.07987713813702</v>
-      </c>
-    </row>
-    <row r="54" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J54" t="s">
         <v>78</v>
       </c>
@@ -4463,17 +6109,8 @@
       <c r="AB54">
         <v>471.68539071083001</v>
       </c>
-      <c r="AH54" t="s">
-        <v>486</v>
-      </c>
-      <c r="AI54">
-        <v>16.524764066273999</v>
-      </c>
-      <c r="AJ54">
-        <v>565.05460000038101</v>
-      </c>
-    </row>
-    <row r="55" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J55" t="s">
         <v>85</v>
       </c>
@@ -4510,17 +6147,8 @@
       <c r="AB55">
         <v>454.53188490867598</v>
       </c>
-      <c r="AH55" t="s">
-        <v>438</v>
-      </c>
-      <c r="AI55">
-        <v>16.584615505206799</v>
-      </c>
-      <c r="AJ55">
-        <v>556.31638860702503</v>
-      </c>
-    </row>
-    <row r="56" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J56" t="s">
         <v>68</v>
       </c>
@@ -4557,17 +6185,8 @@
       <c r="AB56">
         <v>463.87284421920702</v>
       </c>
-      <c r="AH56" t="s">
-        <v>435</v>
-      </c>
-      <c r="AI56">
-        <v>17.0789018707647</v>
-      </c>
-      <c r="AJ56">
-        <v>551.69985389709404</v>
-      </c>
-    </row>
-    <row r="57" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J57" t="s">
         <v>70</v>
       </c>
@@ -4604,17 +6223,8 @@
       <c r="AB57">
         <v>472.76208496093699</v>
       </c>
-      <c r="AH57" t="s">
-        <v>458</v>
-      </c>
-      <c r="AI57">
-        <v>17.1006071374523</v>
-      </c>
-      <c r="AJ57">
-        <v>552.01675868034295</v>
-      </c>
-    </row>
-    <row r="58" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J58" t="s">
         <v>40</v>
       </c>
@@ -4651,17 +6261,8 @@
       <c r="AB58">
         <v>495.68671965598998</v>
       </c>
-      <c r="AH58" t="s">
-        <v>459</v>
-      </c>
-      <c r="AI58">
-        <v>17.344819409618101</v>
-      </c>
-      <c r="AJ58">
-        <v>551.10294508933998</v>
-      </c>
-    </row>
-    <row r="59" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J59" t="s">
         <v>90</v>
       </c>
@@ -4698,17 +6299,8 @@
       <c r="AB59">
         <v>446.59040546417202</v>
       </c>
-      <c r="AH59" t="s">
-        <v>463</v>
-      </c>
-      <c r="AI59">
-        <v>17.5940444204121</v>
-      </c>
-      <c r="AJ59">
-        <v>549.84745550155606</v>
-      </c>
-    </row>
-    <row r="60" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J60" t="s">
         <v>24</v>
       </c>
@@ -4745,17 +6337,8 @@
       <c r="AB60">
         <v>451.53783130645701</v>
       </c>
-      <c r="AH60" t="s">
-        <v>433</v>
-      </c>
-      <c r="AI60">
-        <v>18.008526817819501</v>
-      </c>
-      <c r="AJ60">
-        <v>554.29002285003605</v>
-      </c>
-    </row>
-    <row r="61" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J61" t="s">
         <v>77</v>
       </c>
@@ -4792,17 +6375,8 @@
       <c r="AB61">
         <v>458.28167891502301</v>
       </c>
-      <c r="AH61" t="s">
-        <v>450</v>
-      </c>
-      <c r="AI61">
-        <v>18.5680615134</v>
-      </c>
-      <c r="AJ61">
-        <v>561.67068004608097</v>
-      </c>
-    </row>
-    <row r="62" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J62" t="s">
         <v>73</v>
       </c>
@@ -4839,17 +6413,8 @@
       <c r="AB62">
         <v>466.81496286392201</v>
       </c>
-      <c r="AH62" t="s">
-        <v>476</v>
-      </c>
-      <c r="AI62">
-        <v>18.8296687458914</v>
-      </c>
-      <c r="AJ62">
-        <v>571.00241088867097</v>
-      </c>
-    </row>
-    <row r="63" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J63" t="s">
         <v>5</v>
       </c>
@@ -4886,17 +6451,8 @@
       <c r="AB63">
         <v>466.91864538192698</v>
       </c>
-      <c r="AH63" t="s">
-        <v>414</v>
-      </c>
-      <c r="AI63">
-        <v>19.202660872329499</v>
-      </c>
-      <c r="AJ63">
-        <v>552.21669936180103</v>
-      </c>
-    </row>
-    <row r="64" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J64" t="s">
         <v>81</v>
       </c>
@@ -4933,17 +6489,8 @@
       <c r="AB64">
         <v>430.166829586029</v>
       </c>
-      <c r="AH64" t="s">
-        <v>466</v>
-      </c>
-      <c r="AI64">
-        <v>19.3198065644455</v>
-      </c>
-      <c r="AJ64">
-        <v>607.20337057113602</v>
-      </c>
-    </row>
-    <row r="65" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J65" t="s">
         <v>59</v>
       </c>
@@ -4980,17 +6527,8 @@
       <c r="AB65">
         <v>460.77477574348399</v>
       </c>
-      <c r="AH65" t="s">
-        <v>473</v>
-      </c>
-      <c r="AI65">
-        <v>20.173464699129799</v>
-      </c>
-      <c r="AJ65">
-        <v>604.91599607467595</v>
-      </c>
-    </row>
-    <row r="66" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J66" t="s">
         <v>54</v>
       </c>
@@ -5027,17 +6565,8 @@
       <c r="AB66">
         <v>464.27812075614901</v>
       </c>
-      <c r="AH66" t="s">
-        <v>446</v>
-      </c>
-      <c r="AI66">
-        <v>20.456877708572598</v>
-      </c>
-      <c r="AJ66">
-        <v>552.27368021011296</v>
-      </c>
-    </row>
-    <row r="67" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J67" t="s">
         <v>9</v>
       </c>
@@ -5074,17 +6603,8 @@
       <c r="AB67">
         <v>474.37155032157898</v>
       </c>
-      <c r="AH67" t="s">
-        <v>427</v>
-      </c>
-      <c r="AI67">
-        <v>21.766450407942202</v>
-      </c>
-      <c r="AJ67">
-        <v>539.53674578666596</v>
-      </c>
-    </row>
-    <row r="68" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J68" t="s">
         <v>21</v>
       </c>
@@ -5121,17 +6641,8 @@
       <c r="AB68">
         <v>484.40725684165898</v>
       </c>
-      <c r="AH68" t="s">
-        <v>465</v>
-      </c>
-      <c r="AI68">
-        <v>21.774858031517699</v>
-      </c>
-      <c r="AJ68">
-        <v>552.68054842948902</v>
-      </c>
-    </row>
-    <row r="69" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J69" t="s">
         <v>18</v>
       </c>
@@ -5168,17 +6679,8 @@
       <c r="AB69">
         <v>456.29935860633799</v>
       </c>
-      <c r="AH69" t="s">
-        <v>453</v>
-      </c>
-      <c r="AI69">
-        <v>25.6137153884405</v>
-      </c>
-      <c r="AJ69">
-        <v>547.92505502700806</v>
-      </c>
-    </row>
-    <row r="70" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J70" t="s">
         <v>29</v>
       </c>
@@ -5215,17 +6717,8 @@
       <c r="AB70">
         <v>448.275881290435</v>
       </c>
-      <c r="AH70" t="s">
-        <v>426</v>
-      </c>
-      <c r="AI70">
-        <v>25.759983176010699</v>
-      </c>
-      <c r="AJ70">
-        <v>548.47486281394902</v>
-      </c>
-    </row>
-    <row r="71" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J71" t="s">
         <v>62</v>
       </c>
@@ -5262,17 +6755,8 @@
       <c r="AB71">
         <v>449.72042059898303</v>
       </c>
-      <c r="AH71" t="s">
-        <v>422</v>
-      </c>
-      <c r="AI71">
-        <v>25.859805458524999</v>
-      </c>
-      <c r="AJ71">
-        <v>549.68849158287003</v>
-      </c>
-    </row>
-    <row r="72" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J72" t="s">
         <v>11</v>
       </c>
@@ -5309,17 +6793,8 @@
       <c r="AB72">
         <v>452.45340895652703</v>
       </c>
-      <c r="AH72" t="s">
-        <v>430</v>
-      </c>
-      <c r="AI72">
-        <v>27.172227433090999</v>
-      </c>
-      <c r="AJ72">
-        <v>552.95644927024796</v>
-      </c>
-    </row>
-    <row r="73" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J73" t="s">
         <v>43</v>
       </c>
@@ -5356,17 +6831,8 @@
       <c r="AB73">
         <v>481.52108931541397</v>
       </c>
-      <c r="AH73" t="s">
-        <v>457</v>
-      </c>
-      <c r="AI73">
-        <v>29.530981053831901</v>
-      </c>
-      <c r="AJ73">
-        <v>557.08913278579701</v>
-      </c>
-    </row>
-    <row r="74" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J74" t="s">
         <v>35</v>
       </c>
@@ -5403,17 +6869,8 @@
       <c r="AB74">
         <v>465.93924403190601</v>
       </c>
-      <c r="AH74" t="s">
-        <v>413</v>
-      </c>
-      <c r="AI74">
-        <v>33.959683433887101</v>
-      </c>
-      <c r="AJ74">
-        <v>577.53660178184498</v>
-      </c>
-    </row>
-    <row r="75" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J75" t="s">
         <v>22</v>
       </c>
@@ -5450,17 +6907,8 @@
       <c r="AB75">
         <v>423.12257862091002</v>
       </c>
-      <c r="AH75" t="s">
-        <v>431</v>
-      </c>
-      <c r="AI75">
-        <v>36.347684157767503</v>
-      </c>
-      <c r="AJ75">
-        <v>555.99448037147499</v>
-      </c>
-    </row>
-    <row r="76" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J76" t="s">
         <v>71</v>
       </c>
@@ -5497,17 +6945,8 @@
       <c r="AB76">
         <v>456.338294506073</v>
       </c>
-      <c r="AH76" t="s">
-        <v>417</v>
-      </c>
-      <c r="AI76">
-        <v>36.804735098130898</v>
-      </c>
-      <c r="AJ76">
-        <v>551.35695934295597</v>
-      </c>
-    </row>
-    <row r="77" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J77" t="s">
         <v>82</v>
       </c>
@@ -5544,17 +6983,8 @@
       <c r="AB77">
         <v>457.564157485961</v>
       </c>
-      <c r="AH77" t="s">
-        <v>451</v>
-      </c>
-      <c r="AI77">
-        <v>37.126301279640799</v>
-      </c>
-      <c r="AJ77">
-        <v>549.52855634689297</v>
-      </c>
-    </row>
-    <row r="78" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J78" t="s">
         <v>103</v>
       </c>
@@ -5591,17 +7021,8 @@
       <c r="AB78">
         <v>447.22997760772699</v>
       </c>
-      <c r="AH78" t="s">
-        <v>434</v>
-      </c>
-      <c r="AI78">
-        <v>38.111344808996797</v>
-      </c>
-      <c r="AJ78">
-        <v>557.98984265327397</v>
-      </c>
-    </row>
-    <row r="79" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J79" t="s">
         <v>47</v>
       </c>
@@ -5638,17 +7059,8 @@
       <c r="AB79">
         <v>446.849892377853</v>
       </c>
-      <c r="AH79" t="s">
-        <v>454</v>
-      </c>
-      <c r="AI79">
-        <v>38.265523077921699</v>
-      </c>
-      <c r="AJ79">
-        <v>545.68078470230103</v>
-      </c>
-    </row>
-    <row r="80" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J80" t="s">
         <v>104</v>
       </c>
@@ -5685,17 +7097,8 @@
       <c r="AB80">
         <v>561.52712655067398</v>
       </c>
-      <c r="AH80" t="s">
-        <v>469</v>
-      </c>
-      <c r="AI80">
-        <v>38.273913263176098</v>
-      </c>
-      <c r="AJ80">
-        <v>606.43838500976506</v>
-      </c>
-    </row>
-    <row r="81" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J81" t="s">
         <v>48</v>
       </c>
@@ -5732,17 +7135,8 @@
       <c r="AB81">
         <v>529.68336582183804</v>
       </c>
-      <c r="AH81" t="s">
-        <v>420</v>
-      </c>
-      <c r="AI81">
-        <v>38.634687223298798</v>
-      </c>
-      <c r="AJ81">
-        <v>541.03124713897705</v>
-      </c>
-    </row>
-    <row r="82" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J82" t="s">
         <v>15</v>
       </c>
@@ -5779,17 +7173,8 @@
       <c r="AB82">
         <v>461.50565838813702</v>
       </c>
-      <c r="AH82" t="s">
-        <v>437</v>
-      </c>
-      <c r="AI82">
-        <v>40.605308035185999</v>
-      </c>
-      <c r="AJ82">
-        <v>546.10663652419998</v>
-      </c>
-    </row>
-    <row r="83" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J83" t="s">
         <v>17</v>
       </c>
@@ -5826,17 +7211,8 @@
       <c r="AB83">
         <v>457.39397072792002</v>
       </c>
-      <c r="AH83" t="s">
-        <v>411</v>
-      </c>
-      <c r="AI83">
-        <v>40.836322480580101</v>
-      </c>
-      <c r="AJ83">
-        <v>592.688787221908</v>
-      </c>
-    </row>
-    <row r="84" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J84" t="s">
         <v>100</v>
       </c>
@@ -5873,17 +7249,8 @@
       <c r="AB84">
         <v>444.68302845954798</v>
       </c>
-      <c r="AH84" t="s">
-        <v>470</v>
-      </c>
-      <c r="AI84">
-        <v>48.019770339454098</v>
-      </c>
-      <c r="AJ84">
-        <v>624.087742328643</v>
-      </c>
-    </row>
-    <row r="85" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J85" t="s">
         <v>67</v>
       </c>
@@ -5920,17 +7287,8 @@
       <c r="AB85">
         <v>449.37123632431002</v>
       </c>
-      <c r="AH85" t="s">
-        <v>436</v>
-      </c>
-      <c r="AI85">
-        <v>58.1604207562143</v>
-      </c>
-      <c r="AJ85">
-        <v>553.85716915130604</v>
-      </c>
-    </row>
-    <row r="86" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J86" t="s">
         <v>89</v>
       </c>
@@ -5967,17 +7325,8 @@
       <c r="AB86">
         <v>458.89527630805901</v>
       </c>
-      <c r="AH86" t="s">
-        <v>423</v>
-      </c>
-      <c r="AI86">
-        <v>64.208715115642505</v>
-      </c>
-      <c r="AJ86">
-        <v>534.68929409980694</v>
-      </c>
-    </row>
-    <row r="87" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J87" t="s">
         <v>50</v>
       </c>
@@ -6014,17 +7363,8 @@
       <c r="AB87">
         <v>482.993345975875</v>
       </c>
-      <c r="AH87" t="s">
-        <v>480</v>
-      </c>
-      <c r="AI87">
-        <v>75.910843852579106</v>
-      </c>
-      <c r="AJ87">
-        <v>585.322126150131</v>
-      </c>
-    </row>
-    <row r="88" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J88" t="s">
         <v>84</v>
       </c>
@@ -6061,17 +7401,8 @@
       <c r="AB88">
         <v>454.076018333435</v>
       </c>
-      <c r="AH88" t="s">
-        <v>443</v>
-      </c>
-      <c r="AI88">
-        <v>130.23256751845099</v>
-      </c>
-      <c r="AJ88">
-        <v>557.51699590682904</v>
-      </c>
-    </row>
-    <row r="89" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J89" t="s">
         <v>72</v>
       </c>
@@ -6108,17 +7439,8 @@
       <c r="AB89">
         <v>451.34190487861599</v>
       </c>
-      <c r="AH89" t="s">
-        <v>428</v>
-      </c>
-      <c r="AI89">
-        <v>266.75183048566703</v>
-      </c>
-      <c r="AJ89">
-        <v>540.02358150482098</v>
-      </c>
-    </row>
-    <row r="90" spans="10:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J90" t="s">
         <v>102</v>
       </c>
@@ -6156,7 +7478,7 @@
         <v>442.52571773529002</v>
       </c>
     </row>
-    <row r="91" spans="10:36" x14ac:dyDescent="0.25">
+    <row r="91" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J91" t="s">
         <v>8</v>
       </c>
@@ -6194,7 +7516,7 @@
         <v>459.81624746322598</v>
       </c>
     </row>
-    <row r="92" spans="10:36" x14ac:dyDescent="0.25">
+    <row r="92" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J92" t="s">
         <v>45</v>
       </c>
@@ -6232,7 +7554,7 @@
         <v>456.65805172920199</v>
       </c>
     </row>
-    <row r="93" spans="10:36" x14ac:dyDescent="0.25">
+    <row r="93" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J93" t="s">
         <v>44</v>
       </c>
@@ -6270,7 +7592,7 @@
         <v>454.17499971389702</v>
       </c>
     </row>
-    <row r="94" spans="10:36" x14ac:dyDescent="0.25">
+    <row r="94" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J94" t="s">
         <v>19</v>
       </c>
@@ -6308,7 +7630,7 @@
         <v>458.95745801925602</v>
       </c>
     </row>
-    <row r="95" spans="10:36" x14ac:dyDescent="0.25">
+    <row r="95" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J95" t="s">
         <v>57</v>
       </c>
@@ -6346,7 +7668,7 @@
         <v>588.717991828918</v>
       </c>
     </row>
-    <row r="96" spans="10:36" x14ac:dyDescent="0.25">
+    <row r="96" spans="10:28" x14ac:dyDescent="0.25">
       <c r="J96" t="s">
         <v>95</v>
       </c>
@@ -6994,12 +8316,533 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="5">
+  <tableParts count="7">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B02257E-DF2A-4E2A-867E-821DAC1686C8}">
+  <dimension ref="B3:K24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>427</v>
+      </c>
+      <c r="E3" t="s">
+        <v>428</v>
+      </c>
+      <c r="F3" t="s">
+        <v>307</v>
+      </c>
+      <c r="G3" t="s">
+        <v>308</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>440</v>
+      </c>
+      <c r="J3" t="s">
+        <v>441</v>
+      </c>
+      <c r="K3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>184.77</v>
+      </c>
+      <c r="G4" s="1">
+        <v>107.81</v>
+      </c>
+      <c r="H4" s="1">
+        <v>88</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:I13" si="0">LN(F4*G4)</f>
+        <v>9.8994822269180887</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" ref="J4:J7" si="1">H4*I4</f>
+        <v>871.15443596879186</v>
+      </c>
+      <c r="K4" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>67.23</v>
+      </c>
+      <c r="G5" s="1">
+        <v>56.82</v>
+      </c>
+      <c r="H5" s="1">
+        <v>104</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>8.2480079529069865</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="1"/>
+        <v>857.79282710232656</v>
+      </c>
+      <c r="K5" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>38.075737002891607</v>
+      </c>
+      <c r="G6" s="1">
+        <v>60.441018011152849</v>
+      </c>
+      <c r="H6" s="1">
+        <v>170.38613467454874</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>7.7412452358004424</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="1"/>
+        <v>1319.0008532958029</v>
+      </c>
+      <c r="K6" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>30.435465646657672</v>
+      </c>
+      <c r="G7" s="1">
+        <v>42.872984967778756</v>
+      </c>
+      <c r="H7" s="1">
+        <v>330.41396975040419</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>7.1738504680839243</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="1"/>
+        <v>2370.3404115554049</v>
+      </c>
+      <c r="K7" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>57.663611989875236</v>
+      </c>
+      <c r="G8" s="1">
+        <v>53.408413991848306</v>
+      </c>
+      <c r="H8" s="1">
+        <v>213.82170603990525</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>8.032594632097247</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" ref="J8:J11" si="2">H8*I8</f>
+        <v>1717.5430881620184</v>
+      </c>
+      <c r="K8" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <v>49.42</v>
+      </c>
+      <c r="G9" s="1">
+        <v>41.5</v>
+      </c>
+      <c r="H9" s="1">
+        <v>321</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>7.6260486277971165</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="2"/>
+        <v>2447.9616095228744</v>
+      </c>
+      <c r="K9" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>46.057377165327679</v>
+      </c>
+      <c r="G10" s="1">
+        <v>39.177779337550547</v>
+      </c>
+      <c r="H10" s="1">
+        <v>463.65548329353317</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>7.497997681340979</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="2"/>
+        <v>3476.4877386759426</v>
+      </c>
+      <c r="K10" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1">
+        <v>41.66</v>
+      </c>
+      <c r="G11" s="1">
+        <v>34.56</v>
+      </c>
+      <c r="H11" s="1">
+        <v>646</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2722383797686811</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="2"/>
+        <v>4697.865993330568</v>
+      </c>
+      <c r="K11" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1">
+        <v>88.348388835249494</v>
+      </c>
+      <c r="G12" s="1">
+        <v>51.712982041973994</v>
+      </c>
+      <c r="H12" s="1">
+        <v>591.40521828944838</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>8.4269968157588639</v>
+      </c>
+      <c r="J12" s="3">
+        <f>H12*I12</f>
+        <v>4983.7698913483573</v>
+      </c>
+      <c r="K12" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <v>45.45223578363229</v>
+      </c>
+      <c r="G13" s="1">
+        <v>28.525833152605127</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1860.1847903066159</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>7.1674721146981799</v>
+      </c>
+      <c r="J13" s="3">
+        <f>H13*I13</f>
+        <v>13332.822612708351</v>
+      </c>
+      <c r="K13" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1">
+        <v>73.905803199189606</v>
+      </c>
+      <c r="G14" s="1">
+        <v>68.532048385325467</v>
+      </c>
+      <c r="H14" s="2">
+        <v>937.89995930505825</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" ref="I14" si="3">LN(F14*G14)</f>
+        <v>8.5300928480960092</v>
+      </c>
+      <c r="J14" s="3">
+        <f>H14*I14</f>
+        <v>8000.3737350976153</v>
+      </c>
+      <c r="K14" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15" s="1">
+        <v>101.27</v>
+      </c>
+      <c r="G15" s="1">
+        <v>46.88</v>
+      </c>
+      <c r="H15" s="2">
+        <v>839</v>
+      </c>
+      <c r="I15" s="1">
+        <f>LN(F15*G15)</f>
+        <v>8.4653813626129502</v>
+      </c>
+      <c r="J15" s="3">
+        <f>H15*I15</f>
+        <v>7102.4549632322651</v>
+      </c>
+      <c r="K15" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1">
+        <v>93.6</v>
+      </c>
+      <c r="G16" s="1">
+        <v>53.08</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1334</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" ref="I16" si="4">LN(F16*G16)</f>
+        <v>8.5108305929475527</v>
+      </c>
+      <c r="J16" s="3">
+        <f>H16*I16</f>
+        <v>11353.448010992035</v>
+      </c>
+      <c r="K16" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="2"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>